<commit_message>
added changes to uml
</commit_message>
<xml_diff>
--- a/Projects/Midterm/umls.xlsx
+++ b/Projects/Midterm/umls.xlsx
@@ -1,27 +1,299 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp-git\CMPR131-Group-Work\Projects\Midterm\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081B1F60-D623-4333-BE53-8FD5B6851028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="82">
+  <si>
+    <t>(String) the name of the student</t>
+  </si>
+  <si>
+    <t>Holds the constant array size</t>
+  </si>
+  <si>
+    <t>Constant array of strings for levels of student</t>
+  </si>
+  <si>
+    <t>Holds the integer value for the student level</t>
+  </si>
+  <si>
+    <t>holds the students gpa</t>
+  </si>
+  <si>
+    <t>true if not initialized and empty</t>
+  </si>
+  <si>
+    <t>true if an error occurs</t>
+  </si>
+  <si>
+    <t>debug switch</t>
+  </si>
+  <si>
+    <t>- checkEmpty() void</t>
+  </si>
+  <si>
+    <t>+ student( pName string, pNLevel int, pGpa double )</t>
+  </si>
+  <si>
+    <t>Default constructor declaring an object for the student, intializes the string, int and double to default values if no parameters given</t>
+  </si>
+  <si>
+    <t>+ student(copy student&amp; const )</t>
+  </si>
+  <si>
+    <t>UML assignments:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Itz </t>
+  </si>
+  <si>
+    <t>application</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>vector</t>
+  </si>
+  <si>
+    <t>student</t>
+  </si>
+  <si>
+    <t>done together</t>
+  </si>
+  <si>
+    <t>Tony, Jose</t>
+  </si>
+  <si>
+    <t>Thien</t>
+  </si>
+  <si>
+    <t>+ operator &lt;&lt; (strm ostream&amp;, obj student&amp; const): ostream&amp; friend</t>
+  </si>
+  <si>
+    <t>+ operator &lt;&lt; (strm ostream&amp;, obj student&amp; ): ostream&amp; friend</t>
+  </si>
+  <si>
+    <t>+ operator &gt;&gt; (istream&amp; strm, student&amp; obj): istream&amp; friend</t>
+  </si>
+  <si>
+    <t>Mutators</t>
+  </si>
+  <si>
+    <t>Postcondition: comparing objects of two students by the less than or equal sign</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precondition: (student&amp;) obj is the student object to the right </t>
+  </si>
+  <si>
+    <t>Postcondition: returns true if the gpa, strlevel, and name are all less than or eqaul to the object</t>
+  </si>
+  <si>
+    <t>Postcondition: returns true is the gpa, strlevel, and name are all equal</t>
+  </si>
+  <si>
+    <t>Postcondition: returns true if the error bit is on</t>
+  </si>
+  <si>
+    <t>Postcondition: returns true if the student object is empty</t>
+  </si>
+  <si>
+    <t>Postcondition: returns the gpa of the student</t>
+  </si>
+  <si>
+    <t>Postcondition: returns the integer level of the student</t>
+  </si>
+  <si>
+    <t>Postcondition: returns the string equivalent to the student level</t>
+  </si>
+  <si>
+    <t>Postcondition: returns the name value of the student</t>
+  </si>
+  <si>
+    <t>Postcondition: Copy constructor, copies one student to the next</t>
+  </si>
+  <si>
+    <t>Postcondition: checks if the empty</t>
+  </si>
+  <si>
+    <t>Precondition: (student&amp;) obj is the student object to the right of the comparison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postcondition: returns true if the gpa or the name are less than the object </t>
+  </si>
+  <si>
+    <t>Precondition: (student&amp;) obj is the student object to the right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postcondition: returns true if the gpa or the name are greater than the object </t>
+  </si>
+  <si>
+    <t>Precondition:</t>
+  </si>
+  <si>
+    <t>Postcondition:</t>
+  </si>
+  <si>
+    <t>Student Class UML</t>
+  </si>
+  <si>
+    <t>- mName: int const</t>
+  </si>
+  <si>
+    <t>- LEVELS_ARRSIZE: int const</t>
+  </si>
+  <si>
+    <t>- LEVELS[]: string const</t>
+  </si>
+  <si>
+    <t>- mLevel: int</t>
+  </si>
+  <si>
+    <t>- mGpa: double</t>
+  </si>
+  <si>
+    <t>- mEmpty: bool</t>
+  </si>
+  <si>
+    <t>- mError: bool</t>
+  </si>
+  <si>
+    <t>- DEBUG: bool const</t>
+  </si>
+  <si>
+    <t>+ getName(): const string</t>
+  </si>
+  <si>
+    <t>+ getLevel(): const string</t>
+  </si>
+  <si>
+    <t>+ getNLevel(): const int</t>
+  </si>
+  <si>
+    <t>+ getGpa(): const double</t>
+  </si>
+  <si>
+    <t>+ empty(): const bool</t>
+  </si>
+  <si>
+    <t>+ error(): const bool</t>
+  </si>
+  <si>
+    <t>+ operator == (obj student&amp; const): const bool</t>
+  </si>
+  <si>
+    <t>+ operator &lt;= (obj student&amp; const): const  bool</t>
+  </si>
+  <si>
+    <t>+ operator &gt;= (obj student&amp; const): const bool</t>
+  </si>
+  <si>
+    <t>+ operator &lt; (obj student&amp; const): const bool</t>
+  </si>
+  <si>
+    <t>+ operator &gt; (obj student&amp; const): const bool</t>
+  </si>
+  <si>
+    <t>+ setName( pName string): void</t>
+  </si>
+  <si>
+    <t>+ setLevel(pLevel int): void</t>
+  </si>
+  <si>
+    <t>+ setLevel(pLevel string): void</t>
+  </si>
+  <si>
+    <t>+ setGpa(): void</t>
+  </si>
+  <si>
+    <t>+ setGpa(pGpa double): void</t>
+  </si>
+  <si>
+    <t>+ empty(): bool</t>
+  </si>
+  <si>
+    <t>+ operator ==(obj student&amp; const):  bool</t>
+  </si>
+  <si>
+    <t>+ operator &lt;=(obj student&amp; ):  bool</t>
+  </si>
+  <si>
+    <t>+ operator &gt;=(obj student&amp; ): bool</t>
+  </si>
+  <si>
+    <t>+ operator &lt; (obj student&amp; ): bool</t>
+  </si>
+  <si>
+    <t>+ operator &gt; (obj student&amp; ): bool</t>
+  </si>
+  <si>
+    <t>+ operator = (obj student&amp; const): void</t>
+  </si>
+  <si>
+    <t>+ operator = (obj student&amp; ): void</t>
+  </si>
+  <si>
+    <t>Accessors</t>
+  </si>
+  <si>
+    <t>Friend Functions</t>
+  </si>
+  <si>
+    <t>friend ostream&amp; operator &lt;&lt;(ostream&amp; strm, const student&amp; obj)</t>
+  </si>
+  <si>
+    <t>friend ostream&amp; operator &lt;&lt;(ostream&amp; strm, student&amp; obj)</t>
+  </si>
+  <si>
+    <t>friend istream&amp; operator &gt;&gt;(istream&amp; strm, student&amp; obj)</t>
+  </si>
+  <si>
+    <t>friend fstream&amp; operator &gt;&gt;(fstream&amp; strm, student&amp; obj)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -37,7 +309,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -45,12 +317,168 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +758,610 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="84.21875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60.5546875" style="1" customWidth="1"/>
+    <col min="3" max="13" width="8.88671875" style="1"/>
+    <col min="14" max="14" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.6640625" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="10"/>
+      <c r="B10" s="6"/>
+    </row>
+    <row r="11" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="5"/>
+      <c r="B13" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="5"/>
+      <c r="B21" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="5"/>
+      <c r="B23" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="5"/>
+      <c r="B25" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="5"/>
+      <c r="B27" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="5"/>
+      <c r="B29" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="5"/>
+      <c r="B31" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="5"/>
+      <c r="B33" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="5"/>
+      <c r="B35" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="5"/>
+      <c r="B38" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="5"/>
+      <c r="B40" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="5"/>
+      <c r="B42" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="5"/>
+      <c r="B44" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="5"/>
+      <c r="B46" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="5"/>
+      <c r="B48" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="5"/>
+      <c r="B50" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="5"/>
+      <c r="B52" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="5"/>
+      <c r="B54" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="5"/>
+      <c r="B56" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="5"/>
+      <c r="B58" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="5"/>
+      <c r="B60" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="5"/>
+      <c r="B62" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="5"/>
+      <c r="B64" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" s="5"/>
+      <c r="B66" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" s="3"/>
+      <c r="B68" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B70" s="9"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" s="16"/>
+      <c r="B71" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" s="8"/>
+      <c r="B73" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" s="8"/>
+      <c r="B75" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" s="8"/>
+      <c r="B77" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>